<commit_message>
add data for data-set
</commit_message>
<xml_diff>
--- a/data-set.xlsx
+++ b/data-set.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Level 4\Software Engineering Research Project - SENG 44696\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Level 4\Software Engineering Research Project - SENG 44696\GitRepo\sinhalese_language_racism_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04302BF1-B027-43DA-87AC-A1DC8911EBC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C425B517-BA2D-4A7C-989D-BB8EF4674C02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="normal" sheetId="2" r:id="rId1"/>
     <sheet name="racism" sheetId="1" r:id="rId2"/>
     <sheet name="sexual" sheetId="3" r:id="rId3"/>
+    <sheet name="user Tpes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>පෙට්‍රල් බෝම්බ සමග ඇල්ලූ මුස්ලිම් සැකකරුවන්ට හදිසි නීතිය යටතේ ඇප ලැබුණේ කොහොමද ? නීතිය නැව්වේ කවුද ? බොදු බලය විමසයි ...</t>
   </si>
@@ -249,19 +250,6 @@
     <t>ඔන්න ඕකට පොල් මල් පාරවල් දෙකක් දීපන් පිස්සුව හොඳ වෙන්න 🤣 ලයික් කරලා ශේයා කරලා පේජ් එකට සෙට් වෙන්ඩෝ 🤣</t>
   </si>
   <si>
-    <r>
-      <t>පොන්නයා ඇවිල්ලා </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF1D2129"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>☝️☝️☝️😂</t>
-    </r>
-  </si>
-  <si>
     <t>Edward James Kenway</t>
   </si>
   <si>
@@ -308,12 +296,85 @@
   <si>
     <t>message</t>
   </si>
+  <si>
+    <t>මොහුව දන්නා අය තොරතුරු දෙන්න...</t>
+  </si>
+  <si>
+    <t>mandawala.udeshika</t>
+  </si>
+  <si>
+    <t>මංගලගේ නිරාගමික කොලු රෑන❤️ ආගම : ආදරය ජාතිය : ඒක ඕන නැ 😂</t>
+  </si>
+  <si>
+    <t>මහේෂ් රෙනසර පොන්නයා.</t>
+  </si>
+  <si>
+    <t>Lakshan Perera</t>
+  </si>
+  <si>
+    <t>ගායනයටත් රංගනයටත් එක හා සමාන දස්කම් පෑ ලංකාවේ කලාව නැමති පහන්සිල දල්වන්නට අප්‍රමාණ වෙහෙසක් ගත් ලංකාවෙ හිටපු සුපිරිම කලාකරුවෙක්.. ආදරයට කිව්වෙ තට්ටයා.. ඔබ නැති අඩුව මකාලන්න බෑ.. </t>
+  </si>
+  <si>
+    <t>නිවන්සුව ලැබේවා</t>
+  </si>
+  <si>
+    <t>prabhath.lakmal.505</t>
+  </si>
+  <si>
+    <t>ඇමරිකානු නාවික හමුදාවෙ සෙට් එකක් ලංකාවට ඇවිල්ල කරපු පට්ටම වැඩක්..</t>
+  </si>
+  <si>
+    <t>තවත් වටිනා කලාකරුවෙකු දැයට අහිමි විය.. නිවන්සුව ලැබේවා..</t>
+  </si>
+  <si>
+    <t>ප්‍රවීණ ගායන ශිල්පී රොනී ලීච් මහතා හදිසි හෘදයාබාදයකින් අද උදැසන 1දා අභාවප්‍රාප්ත විය. එතුමා ඔස්ට්‍රේලියාවේ පර්ත් නගරයේ ප්‍රසංගයක් සඳහා පසුගිය සෙනසුරාදා මරියසෙල් ගුනතිලක මහත්මිය සමඟ සහභාගී වි අද සවස ශ්‍රී ලංකාවට එන්න සූදානමින් සිටියා. </t>
+  </si>
+  <si>
+    <t>keerthi.pasquel.583</t>
+  </si>
+  <si>
+    <t>අවංක ආදරේට කරන්න බැරි දෙයක් නැ</t>
+  </si>
+  <si>
+    <t>හිතවත් දමිත් අසංක මල්ලි..... ගායක ගායිකා සංගමය වෙනුවෙන් අප ඔබට සිදුවී ඇති කරදරය පිලිබඳව බෙහෙවින් කණගාටු වෙනවා. ඔබ ගැන සොයා බලන්න මම වැල්ලවාය පොලිස් ස්ථාධිපති ටී.එම්.ජයරත්න මහතාට දුරකථනයෙන් කතා කරා.</t>
+  </si>
+  <si>
+    <t>ඇබරෙන-වදන්-1262682920530101</t>
+  </si>
+  <si>
+    <t>2018 ඔක්තෝබර් මාසේ මමත් .. .අනිල් භාරති ගායන ශිල්පියාත්....එනවා ඇමරිකා එක්සත් ජනපදයට....අපේ ආදරණීය රසිකයන් වෙනුවන් ප්‍රසංග කීපයක් පවත්වන්න... ඉක්මනින් හමුවෙමු...</t>
+  </si>
+  <si>
+    <t>keerthi.pasquel.584</t>
+  </si>
+  <si>
+    <t>User Types</t>
+  </si>
+  <si>
+    <t>Artists</t>
+  </si>
+  <si>
+    <t>ත්‍රිපිටකේ කෙප්ප කියල නේ මූ කියන්නෙ</t>
+  </si>
+  <si>
+    <r>
+      <t>පොන්නයා ඇවිල්ලා </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1D2129"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>☝️☝️☝️😂</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -348,17 +409,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF1D2129"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF1D2129"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF1D2129"/>
       <name val="Arial"/>
@@ -374,6 +424,14 @@
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,8 +451,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -406,18 +465,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -724,54 +784,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="609600" y="5570220"/>
-          <a:ext cx="152400" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="AutoShape 6" descr="https://www.facebook.com/images/emoji.php/v9/fab/1.5/16/1f923.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{357AD561-4381-4A97-8457-7282911CA4E8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="609600" y="5935980"/>
           <a:ext cx="152400" cy="152400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1225,254 +1237,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="168.5546875" customWidth="1"/>
-    <col min="3" max="1026" width="8.5546875"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="168.5546875" style="5" customWidth="1"/>
+    <col min="3" max="1026" width="8.5546875" style="5"/>
+    <col min="1027" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="7"/>
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.8" customHeight="1">
-      <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16.2" customHeight="1">
-      <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="7" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="27.6">
+      <c r="A33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="27.6">
-      <c r="A33" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="B34" s="6"/>
+      <c r="B37" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1486,7 +1570,7 @@
   <dimension ref="A1:AML6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1497,10 +1581,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1536,24 +1620,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="114.21875" customWidth="1"/>
-    <col min="3" max="1026" width="8.5546875"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="114.21875" style="5" customWidth="1"/>
+    <col min="3" max="1026" width="8.5546875" style="5"/>
+    <col min="1027" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1572,16 +1658,58 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="B5" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" display="https://www.facebook.com/profile.php?id=100009146667411&amp;fref=ufi&amp;rc=p" xr:uid="{ED1B7231-7734-4720-8B50-60DBD706AF91}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C9BEFD-1510-4D5D-9F1A-A036ED543911}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add normal message data
</commit_message>
<xml_diff>
--- a/data-set.xlsx
+++ b/data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Level 4\Software Engineering Research Project - SENG 44696\GitRepo\sinhalese_language_racism_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C422B6FA-0AF6-4CBD-BE9D-DC2A76B48628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083C64E5-BB9B-4A6C-A58D-A88C688A7DF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="117">
   <si>
     <t>පෙට්‍රල් බෝම්බ සමග ඇල්ලූ මුස්ලිම් සැකකරුවන්ට හදිසි නීතිය යටතේ ඇප ලැබුණේ කොහොමද ? නීතිය නැව්වේ කවුද ? බොදු බලය විමසයි ...</t>
   </si>
@@ -82,46 +82,6 @@
   </si>
   <si>
     <t>ඊයේ රෑ ඇඩුනේ නැති ටික විතරයි..දුක වැඩි උනාම ඇඩෙන්නෑනේ පට්ට කේන්තියක් එන්නේ</t>
-  </si>
-  <si>
-    <r>
-      <t>මහින්ද යනු බලයබලය වෙනුවෙන් ඕනේ එකෙකු සමග සංසර්ගයේ යෙදීමට දෙවරක් පසුබට නොවෙන එකෙකි</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF1D2129"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>..!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>මහින්ද යනු ලිංගික බෙලහීනතාවය නිසා පීඩාවිදින පුද්ගලයෙකි</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF1D2129"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF1D2129"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ඔහුට තුන් පාරක් කරගැනීමට බැරිය</t>
-    </r>
   </si>
   <si>
     <r>
@@ -259,13 +219,198 @@
     <t>රත්නපුර ගොඩකවෙල මේ ටියුෂන් ගුරාගෙන් දරුවන් ප්‍රවේශම්කරගන්න... ආර්ථික විද්‍යව උගන්වන මොහු සමාජ පිලිකාවකි.. බෞද්ධ විරෝධියකි.. භික්ෂූන්ට  අසභ්‍ය වචනයෙන් බැන වැදුනකි...</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>මොහුව දන්නා අය තොරතුරු දෙන්න...</t>
+  </si>
+  <si>
+    <t>mandawala.udeshika</t>
+  </si>
+  <si>
+    <t>මංගලගේ නිරාගමික කොලු රෑන❤️ ආගම : ආදරය ජාතිය : ඒක ඕන නැ 😂</t>
+  </si>
+  <si>
+    <t>මහේෂ් රෙනසර පොන්නයා.</t>
+  </si>
+  <si>
+    <t>Lakshan Perera</t>
+  </si>
+  <si>
+    <t>ගායනයටත් රංගනයටත් එක හා සමාන දස්කම් පෑ ලංකාවේ කලාව නැමති පහන්සිල දල්වන්නට අප්‍රමාණ වෙහෙසක් ගත් ලංකාවෙ හිටපු සුපිරිම කලාකරුවෙක්.. ආදරයට කිව්වෙ තට්ටයා.. ඔබ නැති අඩුව මකාලන්න බෑ.. </t>
+  </si>
+  <si>
+    <t>නිවන්සුව ලැබේවා</t>
+  </si>
+  <si>
+    <t>prabhath.lakmal.505</t>
+  </si>
+  <si>
+    <t>ඇමරිකානු නාවික හමුදාවෙ සෙට් එකක් ලංකාවට ඇවිල්ල කරපු පට්ටම වැඩක්..</t>
+  </si>
+  <si>
+    <t>තවත් වටිනා කලාකරුවෙකු දැයට අහිමි විය.. නිවන්සුව ලැබේවා..</t>
+  </si>
+  <si>
+    <t>ප්‍රවීණ ගායන ශිල්පී රොනී ලීච් මහතා හදිසි හෘදයාබාදයකින් අද උදැසන 1දා අභාවප්‍රාප්ත විය. එතුමා ඔස්ට්‍රේලියාවේ පර්ත් නගරයේ ප්‍රසංගයක් සඳහා පසුගිය සෙනසුරාදා මරියසෙල් ගුනතිලක මහත්මිය සමඟ සහභාගී වි අද සවස ශ්‍රී ලංකාවට එන්න සූදානමින් සිටියා. </t>
+  </si>
+  <si>
+    <t>keerthi.pasquel.583</t>
+  </si>
+  <si>
+    <t>අවංක ආදරේට කරන්න බැරි දෙයක් නැ</t>
+  </si>
+  <si>
+    <t>හිතවත් දමිත් අසංක මල්ලි..... ගායක ගායිකා සංගමය වෙනුවෙන් අප ඔබට සිදුවී ඇති කරදරය පිලිබඳව බෙහෙවින් කණගාටු වෙනවා. ඔබ ගැන සොයා බලන්න මම වැල්ලවාය පොලිස් ස්ථාධිපති ටී.එම්.ජයරත්න මහතාට දුරකථනයෙන් කතා කරා.</t>
+  </si>
+  <si>
+    <t>ඇබරෙන-වදන්-1262682920530101</t>
+  </si>
+  <si>
+    <t>2018 ඔක්තෝබර් මාසේ මමත් .. .අනිල් භාරති ගායන ශිල්පියාත්....එනවා ඇමරිකා එක්සත් ජනපදයට....අපේ ආදරණීය රසිකයන් වෙනුවන් ප්‍රසංග කීපයක් පවත්වන්න... ඉක්මනින් හමුවෙමු...</t>
+  </si>
+  <si>
+    <t>keerthi.pasquel.584</t>
+  </si>
+  <si>
+    <t>User Types</t>
+  </si>
+  <si>
+    <t>Artists</t>
+  </si>
+  <si>
+    <t>ත්‍රිපිටකේ කෙප්ප කියල නේ මූ කියන්නෙ</t>
+  </si>
+  <si>
+    <t>ශ්‍රී ලාංකේය ගායක ගායිකා සංගමයේ මහා සභා රැස්වීමෙන් අනතුරැව ඒ පිළිබඳව අපේ ශිල්පීන් කීපදෙනෙක් දැක්වූ අදහස්...</t>
+  </si>
+  <si>
+    <t>keerthi.pasquel.585</t>
+  </si>
+  <si>
+    <t>සංවත්සර මහා සභා රැස්වීම ශ්‍රී ලංකේය ගායක ගායිකා සංගමය. 2018-09-24</t>
+  </si>
+  <si>
+    <t>keerthi.pasquel.586</t>
+  </si>
+  <si>
+    <t>උණුසුම් සුබ පැතුම් ඔබට ...තෙරුවන් සරණයි ...!</t>
+  </si>
+  <si>
+    <t>dahammanage.daham</t>
+  </si>
+  <si>
+    <t>පිදුරංගල..... ❤️❤️❤️❤️🙋‍♂️🙋‍♂️ පිදුරංගල පුදබිමේ ඉදලා හෙළුව පෙන්නපු උන්ගේ ජාතකේ හොයන උබලා ..... පිදුරංගල නිජබිමේ අපේ හෙළ වීරත්වය විදහාපාන මේ වීඩියෝව තාම බැලුවේ නැද්ද ....?</t>
+  </si>
+  <si>
+    <t>ආදරෙයි බං උඹලට.... හදවත් මුට්ටියේ දන්කුඩයේන්ම ...❤️❤️❤️❤️🙋‍♂️ --- ඉටි කදුළු ......</t>
+  </si>
+  <si>
+    <t>මට ඇහුම්කන් දෙන්න කිසිම කෙනෙක් නෑ.. දමිත් අසංකගෙ හදවතින්ම කියූ මේ වදන් ටික අහන්න... වීඩියෝ උපුටා ගැනීම - මීට කලින් දැකල නෑ තමයි. වැඩසටහන දෙරණ මා නොවන මම..</t>
+  </si>
+  <si>
+    <t>MusicSajje</t>
+  </si>
+  <si>
+    <t>ලෝක ළමා දිනය අදට යෙදී ඇති අතර "සොඳුරු ළමා ලොව සුරකින්න – වැඩිහිටියනි දෑත දෙන්න" යන්න මෙවර එහි තේමාවයි.</t>
+  </si>
+  <si>
+    <t>answer.lk</t>
+  </si>
+  <si>
+    <t>අද ලෝක ළමා දිනයයි ඇත්තටම අද අපේ රටේ අපේ ළමා පරපුරට සුරක්ෂිත සමාජ ආවරණයක් තිබේද කියා විපරම් කල විට හිතට දැනෙන්නේ හරිම කණගාටුවක් . රටේ හැම තැනම ළමා අපරාධ දුෂණ වලින් පිරි ඉතිරි ගිහින්. තවත් පැත්තකින් ළමා නිවාස තුල පුංචි දරුවෝ විශාල වශයෙන් අනාථාවෙලා .</t>
+  </si>
+  <si>
+    <t>බලන්නකෝ මේක ....</t>
+  </si>
+  <si>
+    <t>ලස්සනයි දහම්</t>
+  </si>
+  <si>
+    <t>anusha.gamaethige</t>
+  </si>
+  <si>
+    <t>අපිට හොරෙන් අපි විකුණන පුදුම රටක් මේක.............</t>
+  </si>
+  <si>
+    <t>Mohothak-Sithanna-2053569848208221</t>
+  </si>
+  <si>
+    <t>කෝවිද හිමි ආච්චිලාගේ කරාබු ගලවයි.......</t>
+  </si>
+  <si>
+    <t>ලැජ්ජ නැතිකම මහ මුදලි කමටත් වඩා ලොකුයි කියන්නෙ මොකද ? සිංහලයෝ එහෙම වෙලා දැන්........</t>
+  </si>
+  <si>
+    <t>මේ පුන්‍යවත් වස් කාලයයි ... ඉස්සර වස් කාලයේදී වැලි මළුවේ ඉදගෙන බණ අහපු හැටි මතක් උනා ..හරිම සුන්දරයි. කටින පින්කමට දවස් හතකට පෙර වැලි මළුවේ බණ ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">වසර දෙකකට පෙර...😥 ---- සංතාප ලතැවුල් ---- සංතාප ලතැවුල් වේදනා හංගා සංවේදනා තනි යහනේ ඉකි බින්දා  සංකල්පනා හිත පාරවා රිද්දා  කදුළු බිදුවල රස පහස වින්දා ... </t>
+  </si>
+  <si>
+    <t>ලස්සනයි නිර්මාණය</t>
+  </si>
+  <si>
+    <t>shiwanka.kumara</t>
+  </si>
+  <si>
+    <t>පාළුවට ගිය ජීවිතය පිළිසකර කර ගන්න හැකිනම් ... බාර දෙන්නම් සදහටම මා නුඹේ නමට ....</t>
+  </si>
+  <si>
+    <t>ක්‍රිකට් වලින් ඇෆ්ගනිස්තානයට පරාද අපි ආර්ථිකයෙන් ඉතියෝපියාවටත් පරාදයි.කොහොමද අවුරුදු 70ක පාලනයේ රග</t>
+  </si>
+  <si>
+    <t>දුකම තමයි අය්යේ..😥😥</t>
+  </si>
+  <si>
+    <t>anusha.surangi.100</t>
+  </si>
+  <si>
+    <t>තිත්ත ඇත්ත</t>
+  </si>
+  <si>
+    <t>ethugala.kaviya</t>
+  </si>
+  <si>
+    <t>ලස්සනයි තෙරුවන් සරනයි</t>
+  </si>
+  <si>
+    <t>Samita Sri Samita Sri</t>
+  </si>
+  <si>
+    <t>මගේ තවත් ගී පදවැලක් ඩුබායි සුපිරි තරුවකගේ හඩින් ලගදීම බලාපොරොත්තු වන්න ..🎤🎤🎤</t>
+  </si>
+  <si>
+    <t>වසර ගනනක් පෙරුම් පුරලත් එක හිතක්.. නැත්නම් ...</t>
+  </si>
+  <si>
+    <t>ඔන්න මගේ රත්තරං යහළුවෝ ...ගොඩක් ආදරය කල මගේ කුළුඳුල් ආදරණීය නවකතාව .... හන්තාන මල්.... ලියල ඉවරයි . හදවතින්ම ඔයාලට තිළිණ කරන්නට අවශ්‍ය වැඩකටයුතු ඔන්න ආරම්භ කලා ... ඉක්මනින්ම ඔයාලා අතරට පත්කරන්න මගේ ආදරණීය යහළුවන් මට ආශිර්වාද කරන්න....</t>
+  </si>
+  <si>
+    <t>කියන්නට ඇති නමුදු .. ලියන්නට බලා හිදී හදවතින්ම බොහෝ විස්තර ඔබ අප වෙනුවෙන් .... ආදරෙයි . ආදරෙයි .. ඉටි කඳුළු ....</t>
+  </si>
+  <si>
+    <t>පූජ්‍ය කාගම සිරිනන්ද හිමි ජාතිය ගැන වේදනාවෙන් පැවසූ වදන්!</t>
+  </si>
+  <si>
+    <t>AnverManatunga</t>
+  </si>
+  <si>
     <r>
       <t>ඕක මහලොකු ප්‍රශ්නයක් නෙමෙයි ඕයි.. ඔන්න බෝල දෙකක් මැද්දෙ තඩි පොල්ලක් තියෙන්නෙ ඇයි කියල ඇහුවනම් අන්න ප්‍රශ්න..</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF1D2129"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>😂😂</t>
@@ -278,83 +423,59 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF1D2129"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>😂😂</t>
     </r>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>මොහුව දන්නා අය තොරතුරු දෙන්න...</t>
-  </si>
-  <si>
-    <t>mandawala.udeshika</t>
-  </si>
-  <si>
-    <t>මංගලගේ නිරාගමික කොලු රෑන❤️ ආගම : ආදරය ජාතිය : ඒක ඕන නැ 😂</t>
-  </si>
-  <si>
-    <t>මහේෂ් රෙනසර පොන්නයා.</t>
-  </si>
-  <si>
-    <t>Lakshan Perera</t>
-  </si>
-  <si>
-    <t>ගායනයටත් රංගනයටත් එක හා සමාන දස්කම් පෑ ලංකාවේ කලාව නැමති පහන්සිල දල්වන්නට අප්‍රමාණ වෙහෙසක් ගත් ලංකාවෙ හිටපු සුපිරිම කලාකරුවෙක්.. ආදරයට කිව්වෙ තට්ටයා.. ඔබ නැති අඩුව මකාලන්න බෑ.. </t>
-  </si>
-  <si>
-    <t>නිවන්සුව ලැබේවා</t>
-  </si>
-  <si>
-    <t>prabhath.lakmal.505</t>
-  </si>
-  <si>
-    <t>ඇමරිකානු නාවික හමුදාවෙ සෙට් එකක් ලංකාවට ඇවිල්ල කරපු පට්ටම වැඩක්..</t>
-  </si>
-  <si>
-    <t>තවත් වටිනා කලාකරුවෙකු දැයට අහිමි විය.. නිවන්සුව ලැබේවා..</t>
-  </si>
-  <si>
-    <t>ප්‍රවීණ ගායන ශිල්පී රොනී ලීච් මහතා හදිසි හෘදයාබාදයකින් අද උදැසන 1දා අභාවප්‍රාප්ත විය. එතුමා ඔස්ට්‍රේලියාවේ පර්ත් නගරයේ ප්‍රසංගයක් සඳහා පසුගිය සෙනසුරාදා මරියසෙල් ගුනතිලක මහත්මිය සමඟ සහභාගී වි අද සවස ශ්‍රී ලංකාවට එන්න සූදානමින් සිටියා. </t>
-  </si>
-  <si>
-    <t>keerthi.pasquel.583</t>
-  </si>
-  <si>
-    <t>අවංක ආදරේට කරන්න බැරි දෙයක් නැ</t>
-  </si>
-  <si>
-    <t>හිතවත් දමිත් අසංක මල්ලි..... ගායක ගායිකා සංගමය වෙනුවෙන් අප ඔබට සිදුවී ඇති කරදරය පිලිබඳව බෙහෙවින් කණගාටු වෙනවා. ඔබ ගැන සොයා බලන්න මම වැල්ලවාය පොලිස් ස්ථාධිපති ටී.එම්.ජයරත්න මහතාට දුරකථනයෙන් කතා කරා.</t>
-  </si>
-  <si>
-    <t>ඇබරෙන-වදන්-1262682920530101</t>
-  </si>
-  <si>
-    <t>2018 ඔක්තෝබර් මාසේ මමත් .. .අනිල් භාරති ගායන ශිල්පියාත්....එනවා ඇමරිකා එක්සත් ජනපදයට....අපේ ආදරණීය රසිකයන් වෙනුවන් ප්‍රසංග කීපයක් පවත්වන්න... ඉක්මනින් හමුවෙමු...</t>
-  </si>
-  <si>
-    <t>keerthi.pasquel.584</t>
-  </si>
-  <si>
-    <t>User Types</t>
-  </si>
-  <si>
-    <t>Artists</t>
-  </si>
-  <si>
-    <t>ත්‍රිපිටකේ කෙප්ප කියල නේ මූ කියන්නෙ</t>
+    <r>
+      <t>වසර පහකට පෙර චුටි මැණිකේ අත්තම්මා එක්ක ...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>❤️</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>මහින්ද යනු බලයබලය වෙනුවෙන් ඕනේ එකෙකු සමග සංසර්ගයේ යෙදීමට දෙවරක් පසුබට නොවෙන එකෙකි</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>..!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>මහින්ද යනු ලිංගික බෙලහීනතාවය නිසා පීඩාවිදින පුද්ගලයෙකි</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ඔහුට තුන් පාරක් කරගැනීමට බැරිය</t>
+    </r>
   </si>
   <si>
     <r>
@@ -363,42 +484,26 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF1D2129"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>☝️☝️☝️😂</t>
     </r>
   </si>
   <si>
-    <t>ශ්‍රී ලාංකේය ගායක ගායිකා සංගමයේ මහා සභා රැස්වීමෙන් අනතුරැව ඒ පිළිබඳව අපේ ශිල්පීන් කීපදෙනෙක් දැක්වූ අදහස්...</t>
-  </si>
-  <si>
-    <t>keerthi.pasquel.585</t>
-  </si>
-  <si>
-    <t>සංවත්සර මහා සභා රැස්වීම ශ්‍රී ලංකේය ගායක ගායිකා සංගමය. 2018-09-24</t>
-  </si>
-  <si>
-    <t>keerthi.pasquel.586</t>
-  </si>
-  <si>
-    <t>උණුසුම් සුබ පැතුම් ඔබට ...තෙරුවන් සරණයි ...!</t>
-  </si>
-  <si>
-    <t>dahammanage.daham</t>
-  </si>
-  <si>
-    <t>පිදුරංගල..... ❤️❤️❤️❤️🙋‍♂️🙋‍♂️ පිදුරංගල පුදබිමේ ඉදලා හෙළුව පෙන්නපු උන්ගේ ජාතකේ හොයන උබලා ..... පිදුරංගල නිජබිමේ අපේ හෙළ වීරත්වය විදහාපාන මේ වීඩියෝව තාම බැලුවේ නැද්ද ....?</t>
-  </si>
-  <si>
-    <t>ආදරෙයි බං උඹලට.... හදවත් මුට්ටියේ දන්කුඩයේන්ම ...❤️❤️❤️❤️🙋‍♂️ --- ඉටි කදුළු ......</t>
+    <t>වස්සාන කාලයට පෙම් බැන්ද බඹරුන්ට  ගිම්හානේ මල් පිපෙන බව නොහැගෙනා දුර ඈත කාලයට අත වනන නුඹේ දෑත සියුමැලි නැතත් මට ප්‍රියේ වාසනා .......</t>
+  </si>
+  <si>
+    <t>ඩුබායි ඉන්න වැලිමඩ SET එකත් එක්ක .... ආදරෙයි ..</t>
+  </si>
+  <si>
+    <t>උසස් හදවත් කවදාවත් පරදින්නේ නෑ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -414,46 +519,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF1D2129"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -462,6 +530,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -483,29 +574,27 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -815,6 +904,54 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="609600" y="5570220"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 3" descr="https://www.facebook.com/images/emoji.php/v9/ff3/1.5/16/2764.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEA4C389-8C16-49F9-B744-DF4F24AAB298}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="11955780"/>
           <a:ext cx="152400" cy="152400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1268,371 +1405,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:A49"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="168.5546875" style="6" customWidth="1"/>
-    <col min="3" max="1026" width="8.5546875" style="6"/>
-    <col min="1027" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="168.5546875" style="4" customWidth="1"/>
+    <col min="3" max="1026" width="8.5546875" style="4"/>
+    <col min="1027" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>51</v>
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="5" spans="1:2">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" customHeight="1">
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.8" customHeight="1">
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16.2" customHeight="1">
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6" customHeight="1">
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="7" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="7" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="7" t="s">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="7" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="6" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="6" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="6" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="7" t="s">
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="27.6">
+      <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="27.6">
-      <c r="A33" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>54</v>
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="10" t="s">
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="8" t="s">
+      <c r="B46" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>82</v>
+      <c r="B74" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A66" r:id="rId1" display="https://www.facebook.com/profile.php?id=100022093120601&amp;fref=ufi" xr:uid="{83B2CCEF-BEAE-4C4C-92EB-D12B08A854CE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1652,10 +2007,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1699,49 +2054,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
-    <col min="2" max="2" width="114.21875" style="6" customWidth="1"/>
-    <col min="3" max="1026" width="8.5546875" style="6"/>
-    <col min="1027" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="114.21875" style="1" customWidth="1"/>
+    <col min="3" max="1026" width="8.5546875" style="1"/>
+    <col min="1027" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1">
+      <c r="B2" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1">
+      <c r="B3" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="1" customFormat="1">
+      <c r="A6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1756,28 +2111,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C9BEFD-1510-4D5D-9F1A-A036ED543911}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="22.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>70</v>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>